<commit_message>
Fix "Positive sign"->"string w/o leading spaces"
</commit_message>
<xml_diff>
--- a/src/zdemo_excel30.w3mi.data.xlsx
+++ b/src/zdemo_excel30.w3mi.data.xlsx
@@ -59,9 +59,6 @@
     <t>Packed</t>
   </si>
   <si>
-    <t>Positive Value</t>
-  </si>
-  <si>
     <t>Positive Value with 10  Digits</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>String</t>
+  </si>
+  <si>
+    <t>String without leading spaces</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
         <v>13</v>
@@ -465,7 +465,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="B3" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>5000.0200000000004</v>
@@ -476,13 +476,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>1234567890.5000000</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>3</v>
@@ -490,13 +490,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>12345678905.000000</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
@@ -504,13 +504,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>123456789050.00000</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
@@ -518,13 +518,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>1234567890500.0000</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -532,13 +532,13 @@
     </row>
     <row r="14" spans="1:5">
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>12345678905000.000</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -546,13 +546,13 @@
     </row>
     <row r="15" spans="1:5">
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>123456789050000.00</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>

</xml_diff>